<commit_message>
chore: modify example tables for test
</commit_message>
<xml_diff>
--- a/ExcelDataExporter.Unity/GameData/$CustomTypes.xlsx
+++ b/ExcelDataExporter.Unity/GameData/$CustomTypes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t xml:space="preserve">namespace=TestGame
 type=custom-type</t>
@@ -39,7 +39,13 @@
     <t xml:space="preserve">count</t>
   </si>
   <si>
+    <t xml:space="preserve">random</t>
+  </si>
+  <si>
     <t xml:space="preserve">int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int[]</t>
   </si>
   <si>
     <t xml:space="preserve">namespace=TestGame.BattleSystem
@@ -217,8 +223,8 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -250,13 +256,19 @@
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="D3" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -282,8 +294,8 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.03515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -294,32 +306,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -335,38 +347,38 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>